<commit_message>
added excel sheet with visualization of measurements
</commit_message>
<xml_diff>
--- a/src/test/resources/measurements.xlsx
+++ b/src/test/resources/measurements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>putListenableAtomicMap</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>ListenableAtomicConcurrentMapComparisonTest</t>
+  </si>
+  <si>
+    <t>putConcurrentListenableMap</t>
   </si>
 </sst>
 </file>
@@ -175,7 +178,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>putAtomicMap</c:v>
+                  <c:v>putConcurrentListenableMap</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -220,28 +223,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4827</c:v>
+                  <c:v>12311</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9534</c:v>
+                  <c:v>24717</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13977</c:v>
+                  <c:v>37593</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18420</c:v>
+                  <c:v>49833</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24885</c:v>
+                  <c:v>63132</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28482</c:v>
+                  <c:v>75218</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31753</c:v>
+                  <c:v>87741</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36779</c:v>
+                  <c:v>100403</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -256,7 +259,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>putListenableAtomicMap</c:v>
+                  <c:v>putAtomicMap</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -301,6 +304,87 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>4827</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9534</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13977</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18420</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24885</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28482</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31753</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36779</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$4:$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>putListenableAtomicMap</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$6:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$6:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
                   <c:v>7847</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -329,25 +413,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="66600320"/>
-        <c:axId val="82315520"/>
+        <c:axId val="67846912"/>
+        <c:axId val="67849216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66600320"/>
+        <c:axId val="67846912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82315520"/>
+        <c:crossAx val="67849216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82315520"/>
+        <c:axId val="67849216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -355,7 +439,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66600320"/>
+        <c:crossAx val="67846912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -379,19 +463,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1323975</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>1552575</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -694,39 +778,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:D13"/>
+  <dimension ref="A2:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E13" sqref="A4:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4">
+    <row r="5" spans="1:5">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -734,13 +822,16 @@
         <v>3907</v>
       </c>
       <c r="C6" s="1">
+        <v>12311</v>
+      </c>
+      <c r="D6" s="1">
         <v>4827</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>7847</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -748,13 +839,16 @@
         <v>7913</v>
       </c>
       <c r="C7" s="1">
+        <v>24717</v>
+      </c>
+      <c r="D7" s="1">
         <v>9534</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>14964</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -762,13 +856,16 @@
         <v>11696</v>
       </c>
       <c r="C8" s="1">
+        <v>37593</v>
+      </c>
+      <c r="D8" s="1">
         <v>13977</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>22616</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -776,13 +873,16 @@
         <v>16667</v>
       </c>
       <c r="C9" s="1">
+        <v>49833</v>
+      </c>
+      <c r="D9" s="1">
         <v>18420</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>29532</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>10</v>
       </c>
@@ -790,13 +890,16 @@
         <v>18917</v>
       </c>
       <c r="C10" s="1">
+        <v>63132</v>
+      </c>
+      <c r="D10" s="1">
         <v>24885</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>36535</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>12</v>
       </c>
@@ -804,13 +907,16 @@
         <v>22786</v>
       </c>
       <c r="C11" s="1">
+        <v>75218</v>
+      </c>
+      <c r="D11" s="1">
         <v>28482</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>43179</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>14</v>
       </c>
@@ -818,13 +924,16 @@
         <v>27144</v>
       </c>
       <c r="C12" s="1">
+        <v>87741</v>
+      </c>
+      <c r="D12" s="1">
         <v>31753</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>51173</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>16</v>
       </c>
@@ -832,9 +941,12 @@
         <v>31172</v>
       </c>
       <c r="C13" s="1">
+        <v>100403</v>
+      </c>
+      <c r="D13" s="1">
         <v>36779</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>58014</v>
       </c>
     </row>

</xml_diff>

<commit_message>
repeated measurements for StampedLock
</commit_message>
<xml_diff>
--- a/src/test/resources/measurements.xlsx
+++ b/src/test/resources/measurements.xlsx
@@ -84,10 +84,13 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="de-DE"/>
   <c:chart>
+    <c:view3D>
+      <c:perspective val="30"/>
+    </c:view3D>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="stacked"/>
+      <c:area3DChart>
+        <c:grouping val="standard"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -178,7 +181,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>putConcurrentListenableMap</c:v>
+                  <c:v>putAtomicMap</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -223,28 +226,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>12311</c:v>
+                  <c:v>4827</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24717</c:v>
+                  <c:v>9534</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37593</c:v>
+                  <c:v>13977</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49833</c:v>
+                  <c:v>18420</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>63132</c:v>
+                  <c:v>24885</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>75218</c:v>
+                  <c:v>28482</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>87741</c:v>
+                  <c:v>31753</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100403</c:v>
+                  <c:v>36779</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -259,7 +262,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>putAtomicMap</c:v>
+                  <c:v>putListenableAtomicMap</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -304,28 +307,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4827</c:v>
+                  <c:v>7847</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9534</c:v>
+                  <c:v>14964</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13977</c:v>
+                  <c:v>22616</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18420</c:v>
+                  <c:v>29532</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24885</c:v>
+                  <c:v>36535</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28482</c:v>
+                  <c:v>43179</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31753</c:v>
+                  <c:v>51173</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36779</c:v>
+                  <c:v>58014</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -340,7 +343,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>putListenableAtomicMap</c:v>
+                  <c:v>putConcurrentListenableMap</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -385,53 +388,53 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>7847</c:v>
+                  <c:v>9646</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14964</c:v>
+                  <c:v>22427</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22616</c:v>
+                  <c:v>31823</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29532</c:v>
+                  <c:v>43571</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36535</c:v>
+                  <c:v>51593</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43179</c:v>
+                  <c:v>60656</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>51173</c:v>
+                  <c:v>68415</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>58014</c:v>
+                  <c:v>83248</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="67846912"/>
-        <c:axId val="67849216"/>
-      </c:lineChart>
+        <c:axId val="93985408"/>
+        <c:axId val="93991296"/>
+        <c:axId val="59260416"/>
+      </c:area3DChart>
       <c:catAx>
-        <c:axId val="67846912"/>
+        <c:axId val="93985408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67849216"/>
+        <c:crossAx val="93991296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67849216"/>
+        <c:axId val="93991296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -439,10 +442,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67846912"/>
+        <c:crossAx val="93985408"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
+      <c:serAx>
+        <c:axId val="59260416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="93991296"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -462,20 +475,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1552575</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -781,7 +794,7 @@
   <dimension ref="A2:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="A4:E13"/>
+      <selection activeCell="A4" sqref="A4:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -802,17 +815,17 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="E5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1">
@@ -822,13 +835,13 @@
         <v>3907</v>
       </c>
       <c r="C6" s="1">
-        <v>12311</v>
+        <v>4827</v>
       </c>
       <c r="D6" s="1">
-        <v>4827</v>
+        <v>7847</v>
       </c>
       <c r="E6" s="1">
-        <v>7847</v>
+        <v>9646</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -839,13 +852,13 @@
         <v>7913</v>
       </c>
       <c r="C7" s="1">
-        <v>24717</v>
+        <v>9534</v>
       </c>
       <c r="D7" s="1">
-        <v>9534</v>
+        <v>14964</v>
       </c>
       <c r="E7" s="1">
-        <v>14964</v>
+        <v>22427</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -856,13 +869,13 @@
         <v>11696</v>
       </c>
       <c r="C8" s="1">
-        <v>37593</v>
+        <v>13977</v>
       </c>
       <c r="D8" s="1">
-        <v>13977</v>
+        <v>22616</v>
       </c>
       <c r="E8" s="1">
-        <v>22616</v>
+        <v>31823</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -873,13 +886,13 @@
         <v>16667</v>
       </c>
       <c r="C9" s="1">
-        <v>49833</v>
+        <v>18420</v>
       </c>
       <c r="D9" s="1">
-        <v>18420</v>
+        <v>29532</v>
       </c>
       <c r="E9" s="1">
-        <v>29532</v>
+        <v>43571</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -890,13 +903,13 @@
         <v>18917</v>
       </c>
       <c r="C10" s="1">
-        <v>63132</v>
+        <v>24885</v>
       </c>
       <c r="D10" s="1">
-        <v>24885</v>
+        <v>36535</v>
       </c>
       <c r="E10" s="1">
-        <v>36535</v>
+        <v>51593</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -907,13 +920,13 @@
         <v>22786</v>
       </c>
       <c r="C11" s="1">
-        <v>75218</v>
+        <v>28482</v>
       </c>
       <c r="D11" s="1">
-        <v>28482</v>
+        <v>43179</v>
       </c>
       <c r="E11" s="1">
-        <v>43179</v>
+        <v>60656</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -924,13 +937,13 @@
         <v>27144</v>
       </c>
       <c r="C12" s="1">
-        <v>87741</v>
+        <v>31753</v>
       </c>
       <c r="D12" s="1">
-        <v>31753</v>
+        <v>51173</v>
       </c>
       <c r="E12" s="1">
-        <v>51173</v>
+        <v>68415</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -941,13 +954,13 @@
         <v>31172</v>
       </c>
       <c r="C13" s="1">
-        <v>100403</v>
+        <v>36779</v>
       </c>
       <c r="D13" s="1">
-        <v>36779</v>
+        <v>58014</v>
       </c>
       <c r="E13" s="1">
-        <v>58014</v>
+        <v>83248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>